<commit_message>
OTreeAlg: successive querying from the current leaf to verify other nodes
</commit_message>
<xml_diff>
--- a/data/Moore_R100.xlsx
+++ b/data/Moore_R100.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="36">
   <si>
     <t>Correct</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>ExtraStates: 1+confirm/identify</t>
+  </si>
+  <si>
+    <t>ExtraStates: 1+confirm/identify+furtherQuerying</t>
   </si>
 </sst>
 </file>
@@ -1081,8 +1084,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="49601536"/>
-        <c:axId val="49677824"/>
+        <c:axId val="12204672"/>
+        <c:axId val="12210560"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1152,11 +1155,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="131892352"/>
-        <c:axId val="49679744"/>
+        <c:axId val="12214272"/>
+        <c:axId val="12212096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="49601536"/>
+        <c:axId val="12204672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1165,7 +1168,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49677824"/>
+        <c:crossAx val="12210560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1173,7 +1176,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="49677824"/>
+        <c:axId val="12210560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1184,12 +1187,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49601536"/>
+        <c:crossAx val="12204672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="49679744"/>
+        <c:axId val="12212096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1217,12 +1220,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131892352"/>
+        <c:crossAx val="12214272"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="131892352"/>
+        <c:axId val="12214272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1231,7 +1234,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49679744"/>
+        <c:crossAx val="12212096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1643,8 +1646,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="212894848"/>
-        <c:axId val="212896384"/>
+        <c:axId val="12266496"/>
+        <c:axId val="12268288"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1714,11 +1717,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="251751040"/>
-        <c:axId val="251749120"/>
+        <c:axId val="12272000"/>
+        <c:axId val="12269824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="212894848"/>
+        <c:axId val="12266496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1727,7 +1730,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="212896384"/>
+        <c:crossAx val="12268288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1735,7 +1738,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="212896384"/>
+        <c:axId val="12268288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1746,12 +1749,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="212894848"/>
+        <c:crossAx val="12266496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="251749120"/>
+        <c:axId val="12269824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1779,12 +1782,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="251751040"/>
+        <c:crossAx val="12272000"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="251751040"/>
+        <c:axId val="12272000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1793,7 +1796,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="251749120"/>
+        <c:crossAx val="12269824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2205,8 +2208,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="14203136"/>
-        <c:axId val="14213120"/>
+        <c:axId val="201297920"/>
+        <c:axId val="201299456"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2276,11 +2279,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="14216576"/>
-        <c:axId val="14214656"/>
+        <c:axId val="201303168"/>
+        <c:axId val="201300992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="14203136"/>
+        <c:axId val="201297920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2289,7 +2292,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="14213120"/>
+        <c:crossAx val="201299456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2297,7 +2300,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="14213120"/>
+        <c:axId val="201299456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2308,12 +2311,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="14203136"/>
+        <c:crossAx val="201297920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="14214656"/>
+        <c:axId val="201300992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2341,12 +2344,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="14216576"/>
+        <c:crossAx val="201303168"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="14216576"/>
+        <c:axId val="201303168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2355,7 +2358,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="14214656"/>
+        <c:crossAx val="201300992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2779,10 +2782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44:H48"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49:H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3950,6 +3953,96 @@
         <v>24</v>
       </c>
     </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44">
+        <v>1783</v>
+      </c>
+      <c r="C44">
+        <v>5496</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>14092</v>
+      </c>
+      <c r="F44" t="s">
+        <v>31</v>
+      </c>
+      <c r="G44" t="s">
+        <v>33</v>
+      </c>
+      <c r="H44" t="s">
+        <v>35</v>
+      </c>
+      <c r="I44" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="B45">
+        <v>1783</v>
+      </c>
+      <c r="C45">
+        <v>5496</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>14092</v>
+      </c>
+      <c r="F45" t="s">
+        <v>31</v>
+      </c>
+      <c r="G45" t="s">
+        <v>33</v>
+      </c>
+      <c r="H45" t="s">
+        <v>35</v>
+      </c>
+      <c r="I45" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>1</v>
+      </c>
+      <c r="B46">
+        <v>12739</v>
+      </c>
+      <c r="C46">
+        <v>5496</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>74320</v>
+      </c>
+      <c r="F46" t="s">
+        <v>31</v>
+      </c>
+      <c r="G46" t="s">
+        <v>33</v>
+      </c>
+      <c r="H46" t="s">
+        <v>35</v>
+      </c>
+      <c r="I46" t="s">
+        <v>23</v>
+      </c>
+      <c r="J46" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>